<commit_message>
Changed for passing test data from excel
</commit_message>
<xml_diff>
--- a/POMTestNg/src/test/resources/testdata/TestData.xlsx
+++ b/POMTestNg/src/test/resources/testdata/TestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\POMTestNG_March2025\POM_TestngFramework\POMTestNg\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57084B6A-2CC8-455C-94EE-08704F7D4EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB14B28-36E1-4E51-A108-0E728BF61E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
+    <sheet name="productimages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -64,13 +65,46 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>searchitem</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>imagecount</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab 10.1</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Macbook</t>
+  </si>
+  <si>
+    <t>MacBook Air</t>
+  </si>
+  <si>
+    <t>iMac</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +116,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -138,6 +180,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -423,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -528,4 +576,68 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED353B4-F37B-4562-8C73-5E5322AB96FF}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>